<commit_message>
Demokratur added, strip down version
</commit_message>
<xml_diff>
--- a/Pirate_List.xlsx
+++ b/Pirate_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cschmitz\Documents\cschmitz_Dokumente\Diverses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099C0356-28DB-412B-91C1-AE5D743D2ADB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4D7F08-054B-4E02-9CF5-30F503AF2615}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28702" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{83B3DFD3-07DF-4D41-B307-4E205D868A5B}"/>
   </bookViews>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
   <si>
     <t>Meine One Piece PiratenCrew</t>
   </si>
   <si>
-    <t>Captain</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -72,12 +69,6 @@
     <t>Wind-frucht (Logia)</t>
   </si>
   <si>
-    <t>2m groß athletisch</t>
-  </si>
-  <si>
-    <t>Steuermann/Navigator</t>
-  </si>
-  <si>
     <t>Weiblich</t>
   </si>
   <si>
@@ -99,13 +90,61 @@
     <t>Kämpft mit einem Bogen. Sehr Naturverbunden. Beherrscht herrausragendes Vorsehungshaki und schwaches Rüstungshaki</t>
   </si>
   <si>
-    <t xml:space="preserve">sehr hübscher und grazieler Körper. Befindet sich meistin ihrer Zentaurengestalt </t>
-  </si>
-  <si>
-    <t>sehr groß massig und extrem stark (Wahlfischmensch)</t>
-  </si>
-  <si>
     <t>kämpft mit seiner enormen körperkraft, beherrscht excelentes Rüstungshaki, und kann geringfügig Meer/Wasser kontrollieren. Im Extremfall kämft er mit einem Riesigen Küchenmesser, erstaunlich schnell.</t>
+  </si>
+  <si>
+    <t>männlich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,75 m. sehr hübscher und grazieler Körper. Befindet sich meistin ihrer Zentaurengestalt </t>
+  </si>
+  <si>
+    <t>2,3 m. mukulös und kräftig</t>
+  </si>
+  <si>
+    <t>2m. athletisch</t>
+  </si>
+  <si>
+    <t>3,5 m. massig und extrem stark (Wahlfischmensch)</t>
+  </si>
+  <si>
+    <t>Kann seinen Körper zu Ketten machen und Ketten spawnen, Beherrscht vorsehungs und Rüstungshaki und hat seine Teufelsfrucht erwäckt.</t>
+  </si>
+  <si>
+    <t>Captain und Steuermann/Navigator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,55 m. dünn und Flink </t>
+  </si>
+  <si>
+    <t>Seine Frucht erlaubt es ihm, jegliche Pflanzen auf fast jedem Boden belibig schnell und gut wachsen zu lassen. Er trägt immer verschiedene Samen herum, und kann heilkäuter wachsen lassen, oder auch ganze Bäume zum Kampf</t>
+  </si>
+  <si>
+    <t>Grow-Frucht (Paramezia)</t>
+  </si>
+  <si>
+    <t>Ketten-Frucht (Paramezia)</t>
+  </si>
+  <si>
+    <t>Shock Wafe</t>
+  </si>
+  <si>
+    <t>Schall-Frucht (Paramezia)</t>
+  </si>
+  <si>
+    <t>1,9m. Voluminöser Körper, trotzdem schnell und stark</t>
+  </si>
+  <si>
+    <t>Er ist der Musiker durch seinen äußerst schönen Gesang, durch seine Täufelsfrucht, kann er mehrstimmig und in jeglichen Tönen singen. Außerdem haben seine Schallwellen eine enorme Zerstörungskraft und Präzision.</t>
+  </si>
+  <si>
+    <t>Vize_Captain/erster Offizier</t>
+  </si>
+  <si>
+    <t>weiblich</t>
+  </si>
+  <si>
+    <t>1,9 m. schlank, muskulös, hübsch aber gefährlich</t>
   </si>
 </sst>
 </file>
@@ -150,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -160,6 +199,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,13 +519,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358A23CA-7FF5-4BD3-A6AA-BD61631078DD}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.90625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56" customWidth="1"/>
   </cols>
   <sheetData>
@@ -498,84 +540,88 @@
     </row>
     <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>17</v>
+      <c r="A15" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B15" s="1"/>
     </row>
@@ -584,163 +630,189 @@
     </row>
     <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B30" s="1"/>
     </row>
     <row r="31" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B37" s="1"/>
     </row>
     <row r="38" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="1"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B39" s="1"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -748,46 +820,46 @@
     </row>
     <row r="45" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B45" s="1"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B46" s="1"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>